<commit_message>
se añadieron ciudades AMB 2020
se añadió información de población para las ciudades del AMB según la proyección DANE 2020
</commit_message>
<xml_diff>
--- a/data/PoblacionCiudades.xlsx
+++ b/data/PoblacionCiudades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DescargasChrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8C9AB02-A6A8-4AFF-BEB6-B3B1EA290D12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEAF487-AFD5-4B91-94CF-213C361F1A17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4560" windowWidth="20730" windowHeight="11160" xr2:uid="{E6E31D99-B7C3-4591-91DD-A3327547AB8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6E31D99-B7C3-4591-91DD-A3327547AB8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ciudad</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>BELLO</t>
+  </si>
+  <si>
+    <t>FLORIDABLANCA</t>
+  </si>
+  <si>
+    <t>GIRON</t>
+  </si>
+  <si>
+    <t>PIEDECUESTA</t>
   </si>
 </sst>
 </file>
@@ -428,15 +437,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735B5161-D3A1-41A8-A60B-0B0295A3CF9C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -527,6 +538,30 @@
         <v>552154</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>307896</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>171904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>182959</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>